<commit_message>
Clean Version ReadXml and New Card
Version Corigée avec lecture XML et nouveau visuel des cartes
</commit_message>
<xml_diff>
--- a/GameDesign/Templates_Organisation_G4.xlsx
+++ b/GameDesign/Templates_Organisation_G4.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Design" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Général!$A$1:$I$205</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Général!$A$1:$I$204</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="474">
   <si>
     <t>Feature</t>
   </si>
@@ -1181,6 +1181,9 @@
     <t>Socle pour les cartes</t>
   </si>
   <si>
+    <t>icon_socle</t>
+  </si>
+  <si>
     <t>icon_Time</t>
   </si>
   <si>
@@ -1443,15 +1446,6 @@
   </si>
   <si>
     <t>code_controls</t>
-  </si>
-  <si>
-    <t>icon_socle_turn</t>
-  </si>
-  <si>
-    <t>icon_socle_card</t>
-  </si>
-  <si>
-    <t>Socle pour le message qui indique le tour</t>
   </si>
 </sst>
 </file>
@@ -2453,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I213"/>
+  <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2617,10 +2611,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="2"/>
@@ -2640,10 +2634,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="2"/>
@@ -3139,7 +3133,7 @@
         <v>8</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>369</v>
@@ -3244,7 +3238,9 @@
       <c r="I33" s="86"/>
     </row>
     <row r="34" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="66"/>
+      <c r="A34" s="66" t="s">
+        <v>344</v>
+      </c>
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
@@ -3252,14 +3248,16 @@
         <v>8</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>473</v>
+        <v>385</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>475</v>
+        <v>384</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="5"/>
-      <c r="H34" s="17"/>
+      <c r="H34" s="17">
+        <v>0</v>
+      </c>
       <c r="I34" s="99" t="s">
         <v>333</v>
       </c>
@@ -3275,10 +3273,10 @@
         <v>8</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>474</v>
+        <v>387</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="5"/>
@@ -3293,26 +3291,24 @@
       <c r="A36" s="66" t="s">
         <v>344</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>387</v>
+      <c r="B36" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="51" t="s">
+        <v>394</v>
+      </c>
+      <c r="E36" s="51" t="s">
+        <v>396</v>
       </c>
       <c r="F36" s="18"/>
-      <c r="G36" s="5"/>
+      <c r="G36" s="45"/>
       <c r="H36" s="17">
         <v>0</v>
       </c>
-      <c r="I36" s="99" t="s">
-        <v>333</v>
-      </c>
+      <c r="I36" s="89"/>
     </row>
     <row r="37" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="66" t="s">
@@ -3348,10 +3344,10 @@
         <v>8</v>
       </c>
       <c r="D38" s="51" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="45"/>
@@ -3371,10 +3367,10 @@
         <v>8</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="E39" s="51" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="45"/>
@@ -3394,10 +3390,10 @@
         <v>8</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="E40" s="51" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="45"/>
@@ -3417,10 +3413,10 @@
         <v>8</v>
       </c>
       <c r="D41" s="51" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="E41" s="51" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="45"/>
@@ -3440,10 +3436,10 @@
         <v>8</v>
       </c>
       <c r="D42" s="51" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="E42" s="51" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="45"/>
@@ -3463,12 +3459,14 @@
         <v>8</v>
       </c>
       <c r="D43" s="51" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="E43" s="51" t="s">
-        <v>409</v>
-      </c>
-      <c r="F43" s="18"/>
+        <v>414</v>
+      </c>
+      <c r="F43" s="103">
+        <v>1</v>
+      </c>
       <c r="G43" s="45"/>
       <c r="H43" s="17">
         <v>0</v>
@@ -3486,14 +3484,12 @@
         <v>8</v>
       </c>
       <c r="D44" s="51" t="s">
-        <v>412</v>
+        <v>435</v>
       </c>
       <c r="E44" s="51" t="s">
-        <v>413</v>
-      </c>
-      <c r="F44" s="103">
-        <v>1</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="F44" s="16"/>
       <c r="G44" s="45"/>
       <c r="H44" s="17">
         <v>0</v>
@@ -3511,12 +3507,12 @@
         <v>8</v>
       </c>
       <c r="D45" s="51" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="E45" s="51" t="s">
-        <v>435</v>
-      </c>
-      <c r="F45" s="16"/>
+        <v>412</v>
+      </c>
+      <c r="F45" s="18"/>
       <c r="G45" s="45"/>
       <c r="H45" s="17">
         <v>0</v>
@@ -3527,20 +3523,20 @@
       <c r="A46" s="66" t="s">
         <v>344</v>
       </c>
-      <c r="B46" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="C46" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="51" t="s">
-        <v>410</v>
-      </c>
-      <c r="E46" s="51" t="s">
-        <v>411</v>
+      <c r="B46" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>418</v>
       </c>
       <c r="F46" s="18"/>
-      <c r="G46" s="45"/>
+      <c r="G46" s="3"/>
       <c r="H46" s="17">
         <v>0</v>
       </c>
@@ -3557,10 +3553,10 @@
         <v>8</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="3"/>
@@ -3580,10 +3576,10 @@
         <v>8</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F48" s="18"/>
       <c r="G48" s="3"/>
@@ -3603,40 +3599,40 @@
         <v>8</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>416</v>
+        <v>433</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>419</v>
+        <v>434</v>
       </c>
       <c r="F49" s="18"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="17">
-        <v>0</v>
-      </c>
-      <c r="I49" s="89"/>
+      <c r="H49" s="38">
+        <v>0</v>
+      </c>
+      <c r="I49" s="87"/>
     </row>
     <row r="50" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="66" t="s">
         <v>344</v>
       </c>
-      <c r="B50" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>433</v>
+      <c r="B50" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>427</v>
       </c>
       <c r="F50" s="18"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="38">
-        <v>0</v>
-      </c>
-      <c r="I50" s="87"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="17">
+        <v>0</v>
+      </c>
+      <c r="I50" s="86"/>
     </row>
     <row r="51" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="66" t="s">
@@ -3648,14 +3644,14 @@
       <c r="C51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>426</v>
+      <c r="D51" s="101" t="s">
+        <v>422</v>
+      </c>
+      <c r="E51" s="105" t="s">
+        <v>428</v>
       </c>
       <c r="F51" s="18"/>
-      <c r="G51" s="2"/>
+      <c r="G51" s="101"/>
       <c r="H51" s="17">
         <v>0</v>
       </c>
@@ -3672,10 +3668,10 @@
         <v>8</v>
       </c>
       <c r="D52" s="101" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="E52" s="105" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="F52" s="18"/>
       <c r="G52" s="101"/>
@@ -3695,10 +3691,10 @@
         <v>8</v>
       </c>
       <c r="D53" s="101" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="E53" s="105" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="F53" s="18"/>
       <c r="G53" s="101"/>
@@ -3718,10 +3714,10 @@
         <v>8</v>
       </c>
       <c r="D54" s="101" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="E54" s="105" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="F54" s="18"/>
       <c r="G54" s="101"/>
@@ -3741,16 +3737,14 @@
         <v>8</v>
       </c>
       <c r="D55" s="101" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E55" s="105" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="F55" s="18"/>
       <c r="G55" s="101"/>
-      <c r="H55" s="17">
-        <v>0</v>
-      </c>
+      <c r="H55" s="39"/>
       <c r="I55" s="86"/>
     </row>
     <row r="56" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3763,91 +3757,83 @@
       <c r="C56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="101" t="s">
-        <v>425</v>
-      </c>
-      <c r="E56" s="105" t="s">
-        <v>431</v>
-      </c>
-      <c r="F56" s="18"/>
+      <c r="D56" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="F56" s="102"/>
       <c r="G56" s="101"/>
-      <c r="H56" s="39">
-        <v>0</v>
-      </c>
+      <c r="H56" s="39"/>
       <c r="I56" s="86"/>
     </row>
-    <row r="57" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="66" t="s">
+    <row r="57" spans="1:9" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="107" t="s">
         <v>344</v>
       </c>
-      <c r="B57" s="101" t="s">
+      <c r="B57" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="C57" s="104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="100" t="s">
+        <v>392</v>
+      </c>
+      <c r="E57" s="100" t="s">
         <v>390</v>
       </c>
-      <c r="E57" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="F57" s="102"/>
-      <c r="G57" s="101"/>
-      <c r="H57" s="39">
-        <v>0</v>
-      </c>
-      <c r="I57" s="86"/>
-    </row>
-    <row r="58" spans="1:9" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="107" t="s">
-        <v>344</v>
-      </c>
-      <c r="B58" s="106" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="104" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="100" t="s">
-        <v>391</v>
-      </c>
-      <c r="E58" s="100" t="s">
-        <v>389</v>
-      </c>
-      <c r="F58" s="17"/>
-      <c r="G58" s="100"/>
-      <c r="H58" s="112">
-        <v>0</v>
-      </c>
-      <c r="I58" s="90"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
-        <v>436</v>
+      <c r="F57" s="17"/>
+      <c r="G57" s="100"/>
+      <c r="H57" s="112"/>
+      <c r="I57" s="90"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" s="111" t="s">
+        <v>438</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="F58" s="110"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="109"/>
+      <c r="I58" s="88"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="66" t="s">
+        <v>437</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="25" t="s">
+      <c r="C59" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D59" s="111" t="s">
-        <v>437</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="F59" s="110"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="109">
-        <v>0</v>
-      </c>
-      <c r="I59" s="88"/>
+      <c r="D59" s="42" t="s">
+        <v>440</v>
+      </c>
+      <c r="E59" s="42" t="s">
+        <v>441</v>
+      </c>
+      <c r="F59" s="16"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="91"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>6</v>
@@ -3855,45 +3841,41 @@
       <c r="C60" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D60" s="42" t="s">
-        <v>439</v>
-      </c>
-      <c r="E60" s="42" t="s">
-        <v>440</v>
+      <c r="D60" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>443</v>
       </c>
       <c r="F60" s="16"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="17">
-        <v>0</v>
-      </c>
+      <c r="H60" s="17"/>
       <c r="I60" s="91"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="66" t="s">
-        <v>436</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B61" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="F61" s="16"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="17">
-        <v>0</v>
-      </c>
-      <c r="I61" s="91"/>
+      <c r="D61" s="45" t="s">
+        <v>438</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>446</v>
+      </c>
+      <c r="F61" s="18"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="92"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B62" s="45" t="s">
         <v>138</v>
@@ -3902,21 +3884,19 @@
         <v>139</v>
       </c>
       <c r="D62" s="45" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="E62" s="46" t="s">
         <v>445</v>
       </c>
       <c r="F62" s="18"/>
       <c r="G62" s="45"/>
-      <c r="H62" s="16">
-        <v>0</v>
-      </c>
+      <c r="H62" s="18"/>
       <c r="I62" s="92"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B63" s="45" t="s">
         <v>138</v>
@@ -3925,21 +3905,19 @@
         <v>139</v>
       </c>
       <c r="D63" s="45" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="E63" s="46" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="F63" s="18"/>
       <c r="G63" s="45"/>
-      <c r="H63" s="18">
-        <v>0</v>
-      </c>
+      <c r="H63" s="18"/>
       <c r="I63" s="92"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B64" s="45" t="s">
         <v>138</v>
@@ -3948,21 +3926,19 @@
         <v>139</v>
       </c>
       <c r="D64" s="45" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="E64" s="46" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="F64" s="18"/>
       <c r="G64" s="45"/>
-      <c r="H64" s="18">
-        <v>0</v>
-      </c>
+      <c r="H64" s="18"/>
       <c r="I64" s="92"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B65" s="45" t="s">
         <v>138</v>
@@ -3971,21 +3947,19 @@
         <v>139</v>
       </c>
       <c r="D65" s="45" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="E65" s="46" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F65" s="18"/>
       <c r="G65" s="45"/>
-      <c r="H65" s="18">
-        <v>0</v>
-      </c>
+      <c r="H65" s="18"/>
       <c r="I65" s="92"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B66" s="45" t="s">
         <v>138</v>
@@ -3994,21 +3968,19 @@
         <v>139</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E66" s="46" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F66" s="18"/>
       <c r="G66" s="45"/>
-      <c r="H66" s="18">
-        <v>0</v>
-      </c>
+      <c r="H66" s="18"/>
       <c r="I66" s="92"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B67" s="45" t="s">
         <v>138</v>
@@ -4017,67 +3989,61 @@
         <v>139</v>
       </c>
       <c r="D67" s="45" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="E67" s="46" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="F67" s="18"/>
       <c r="G67" s="45"/>
-      <c r="H67" s="18">
-        <v>0</v>
-      </c>
+      <c r="H67" s="18"/>
       <c r="I67" s="92"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="66" t="s">
-        <v>436</v>
-      </c>
-      <c r="B68" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="C68" s="45" t="s">
+        <v>437</v>
+      </c>
+      <c r="B68" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D68" s="45" t="s">
-        <v>451</v>
-      </c>
-      <c r="E68" s="46" t="s">
-        <v>452</v>
+      <c r="D68" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="E68" s="49" t="s">
+        <v>457</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="45"/>
-      <c r="H68" s="18">
-        <v>0</v>
-      </c>
+      <c r="H68" s="18"/>
       <c r="I68" s="92"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="66" t="s">
-        <v>436</v>
-      </c>
-      <c r="B69" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C69" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>453</v>
-      </c>
-      <c r="E69" s="49" t="s">
-        <v>456</v>
+        <v>437</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>459</v>
       </c>
       <c r="F69" s="18"/>
-      <c r="G69" s="45"/>
-      <c r="H69" s="18">
-        <v>0</v>
-      </c>
+      <c r="G69" s="101"/>
+      <c r="H69" s="18"/>
       <c r="I69" s="92"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>9</v>
@@ -4086,21 +4052,19 @@
         <v>8</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="F70" s="18"/>
       <c r="G70" s="101"/>
-      <c r="H70" s="18">
-        <v>0</v>
-      </c>
+      <c r="H70" s="18"/>
       <c r="I70" s="92"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="66" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>9</v>
@@ -4109,253 +4073,210 @@
         <v>8</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="F71" s="18"/>
       <c r="G71" s="101"/>
-      <c r="H71" s="18">
-        <v>0</v>
-      </c>
+      <c r="H71" s="18"/>
       <c r="I71" s="92"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="66" t="s">
-        <v>436</v>
-      </c>
-      <c r="B72" s="2" t="s">
+    <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="108" t="s">
+        <v>437</v>
+      </c>
+      <c r="B72" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="C72" s="104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="104" t="s">
+        <v>391</v>
+      </c>
+      <c r="E72" s="104" t="s">
+        <v>389</v>
+      </c>
+      <c r="F72" s="19"/>
+      <c r="G72" s="100"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="93"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="111" t="s">
+        <v>465</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="F73" s="18"/>
+      <c r="G73" s="111"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="92"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="66" t="s">
+        <v>464</v>
+      </c>
+      <c r="B74" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D74" s="45" t="s">
+        <v>467</v>
+      </c>
+      <c r="E74" s="46" t="s">
+        <v>468</v>
+      </c>
+      <c r="F74" s="18"/>
+      <c r="G74" s="45"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="92"/>
+    </row>
+    <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="108" t="s">
+        <v>464</v>
+      </c>
+      <c r="B75" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="100" t="s">
         <v>462</v>
       </c>
-      <c r="F72" s="18"/>
-      <c r="G72" s="101"/>
-      <c r="H72" s="18">
-        <v>0</v>
-      </c>
-      <c r="I72" s="92"/>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="108" t="s">
-        <v>436</v>
-      </c>
-      <c r="B73" s="104" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="104" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="104" t="s">
-        <v>390</v>
-      </c>
-      <c r="E73" s="104" t="s">
-        <v>388</v>
-      </c>
-      <c r="F73" s="19"/>
-      <c r="G73" s="100"/>
-      <c r="H73" s="19">
-        <v>0</v>
-      </c>
-      <c r="I73" s="93"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
+      <c r="E75" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="F75" s="114"/>
+      <c r="G75" s="113"/>
+      <c r="H75" s="115"/>
+      <c r="I75" s="116"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="B76" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="F76" s="18"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="92"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="D74" s="111" t="s">
-        <v>464</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="F74" s="18"/>
-      <c r="G74" s="111"/>
-      <c r="H74" s="18">
-        <v>0</v>
-      </c>
-      <c r="I74" s="92"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="66" t="s">
-        <v>463</v>
-      </c>
-      <c r="B75" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="C75" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="D75" s="45" t="s">
-        <v>466</v>
-      </c>
-      <c r="E75" s="46" t="s">
-        <v>467</v>
-      </c>
-      <c r="F75" s="18"/>
-      <c r="G75" s="45"/>
-      <c r="H75" s="18">
-        <v>0</v>
-      </c>
-      <c r="I75" s="92"/>
-    </row>
-    <row r="76" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="108" t="s">
-        <v>463</v>
-      </c>
-      <c r="B76" s="100" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="100" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="100" t="s">
-        <v>461</v>
-      </c>
-      <c r="E76" s="100" t="s">
-        <v>462</v>
-      </c>
-      <c r="F76" s="114"/>
-      <c r="G76" s="113"/>
-      <c r="H76" s="115">
-        <v>0</v>
-      </c>
-      <c r="I76" s="116"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="B77" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="E77" s="5" t="s">
+      <c r="D77" s="45" t="s">
+        <v>471</v>
+      </c>
+      <c r="E77" s="45" t="s">
         <v>469</v>
       </c>
       <c r="F77" s="18"/>
       <c r="G77" s="45"/>
-      <c r="H77" s="18">
-        <v>0</v>
-      </c>
+      <c r="H77" s="18"/>
       <c r="I77" s="92"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="22"/>
-      <c r="B78" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="C78" s="45" t="s">
+      <c r="A78" s="66" t="s">
+        <v>311</v>
+      </c>
+      <c r="B78" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="D78" s="45" t="s">
-        <v>470</v>
-      </c>
-      <c r="E78" s="45" t="s">
-        <v>468</v>
-      </c>
-      <c r="F78" s="18"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="18">
-        <v>0</v>
-      </c>
-      <c r="I78" s="92"/>
+      <c r="D78" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="E78" s="51" t="s">
+        <v>315</v>
+      </c>
+      <c r="F78" s="16"/>
+      <c r="G78" s="51"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="91"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="66" t="s">
         <v>311</v>
       </c>
-      <c r="B79" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="C79" s="51" t="s">
+      <c r="B79" s="64" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="D79" s="51" t="s">
-        <v>471</v>
-      </c>
-      <c r="E79" s="51" t="s">
-        <v>315</v>
-      </c>
-      <c r="F79" s="16"/>
-      <c r="G79" s="51"/>
-      <c r="H79" s="16">
-        <v>0</v>
-      </c>
-      <c r="I79" s="91"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="66" t="s">
+      <c r="D79" s="64" t="s">
+        <v>455</v>
+      </c>
+      <c r="E79" s="64" t="s">
+        <v>320</v>
+      </c>
+      <c r="F79" s="61"/>
+      <c r="G79" s="64"/>
+      <c r="H79" s="61"/>
+      <c r="I79" s="94"/>
+    </row>
+    <row r="80" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="67" t="s">
         <v>311</v>
       </c>
-      <c r="B80" s="64" t="s">
-        <v>138</v>
-      </c>
-      <c r="C80" s="64" t="s">
+      <c r="B80" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="D80" s="64" t="s">
-        <v>454</v>
-      </c>
-      <c r="E80" s="64" t="s">
-        <v>320</v>
-      </c>
-      <c r="F80" s="61"/>
-      <c r="G80" s="64"/>
-      <c r="H80" s="61">
-        <v>0</v>
-      </c>
-      <c r="I80" s="94"/>
-    </row>
-    <row r="81" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="67" t="s">
-        <v>311</v>
-      </c>
-      <c r="B81" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="C81" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="D81" s="47" t="s">
-        <v>472</v>
-      </c>
-      <c r="E81" s="47" t="s">
+      <c r="D80" s="47" t="s">
+        <v>473</v>
+      </c>
+      <c r="E80" s="47" t="s">
         <v>317</v>
       </c>
-      <c r="F81" s="19"/>
-      <c r="G81" s="47"/>
-      <c r="H81" s="19">
-        <v>0</v>
-      </c>
-      <c r="I81" s="93"/>
-    </row>
-    <row r="82" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F213" s="32"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="47"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="93"/>
+    </row>
+    <row r="81" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F212" s="32"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H111">
+  <conditionalFormatting sqref="H110">
     <cfRule type="iconSet" priority="13">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -4364,7 +4285,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H132:H133">
+  <conditionalFormatting sqref="H131:H132">
     <cfRule type="iconSet" priority="11">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -4373,7 +4294,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H134:H205 H88:H123 H129:H131">
+  <conditionalFormatting sqref="H133:H204 H87:H122 H128:H130">
     <cfRule type="iconSet" priority="22">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -4382,7 +4303,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H124:H128">
+  <conditionalFormatting sqref="H123:H127">
     <cfRule type="iconSet" priority="7">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -4400,7 +4321,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61:H85">
+  <conditionalFormatting sqref="H60:H84">
     <cfRule type="iconSet" priority="40">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -4409,7 +4330,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H205">
+  <conditionalFormatting sqref="H2:H204">
     <cfRule type="iconSet" priority="42">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -4702,7 +4623,7 @@
       <c r="F11" s="18"/>
       <c r="G11" s="5"/>
       <c r="H11" s="18">
-        <f>Général!H87</f>
+        <f>Général!H86</f>
         <v>0</v>
       </c>
       <c r="I11" s="85"/>
@@ -4726,7 +4647,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="1"/>
       <c r="H12" s="18">
-        <f>Général!H88</f>
+        <f>Général!H87</f>
         <v>0</v>
       </c>
       <c r="I12" s="85"/>
@@ -4750,7 +4671,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="1"/>
       <c r="H13" s="18">
-        <f>Général!H89</f>
+        <f>Général!H88</f>
         <v>0</v>
       </c>
       <c r="I13" s="85"/>
@@ -4774,7 +4695,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="1"/>
       <c r="H14" s="18">
-        <f>Général!H90</f>
+        <f>Général!H89</f>
         <v>0</v>
       </c>
       <c r="I14" s="85"/>
@@ -4798,7 +4719,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="1"/>
       <c r="H15" s="18">
-        <f>Général!H91</f>
+        <f>Général!H90</f>
         <v>0</v>
       </c>
       <c r="I15" s="85"/>
@@ -4822,7 +4743,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="1"/>
       <c r="H16" s="18">
-        <f>Général!H92</f>
+        <f>Général!H91</f>
         <v>0</v>
       </c>
       <c r="I16" s="85"/>
@@ -4846,7 +4767,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="33"/>
       <c r="H17" s="53">
-        <f>Général!H93</f>
+        <f>Général!H92</f>
         <v>0</v>
       </c>
       <c r="I17" s="85"/>
@@ -4870,7 +4791,7 @@
       <c r="F18" s="18"/>
       <c r="G18" s="5"/>
       <c r="H18" s="75">
-        <f>Général!H106</f>
+        <f>Général!H105</f>
         <v>0</v>
       </c>
       <c r="I18" s="85"/>
@@ -4894,7 +4815,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="33"/>
       <c r="H19" s="19">
-        <f>Général!H107</f>
+        <f>Général!H106</f>
         <v>0</v>
       </c>
       <c r="I19" s="85"/>
@@ -4918,7 +4839,7 @@
       <c r="F20" s="53"/>
       <c r="G20" s="42"/>
       <c r="H20" s="53">
-        <f>Général!H121</f>
+        <f>Général!H120</f>
         <v>0</v>
       </c>
       <c r="I20" s="85"/>
@@ -4942,7 +4863,7 @@
       <c r="F21" s="50"/>
       <c r="G21" s="7"/>
       <c r="H21" s="75">
-        <f>Général!H140</f>
+        <f>Général!H139</f>
         <v>0</v>
       </c>
       <c r="I21" s="85"/>
@@ -4966,7 +4887,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="1"/>
       <c r="H22" s="16">
-        <f>Général!H141</f>
+        <f>Général!H140</f>
         <v>0</v>
       </c>
       <c r="I22" s="85"/>
@@ -4990,7 +4911,7 @@
       <c r="F23" s="18"/>
       <c r="G23" s="1"/>
       <c r="H23" s="53">
-        <f>Général!H142</f>
+        <f>Général!H141</f>
         <v>0</v>
       </c>
       <c r="I23" s="85"/>
@@ -5014,7 +4935,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="1"/>
       <c r="H24" s="16">
-        <f>Général!H143</f>
+        <f>Général!H142</f>
         <v>0</v>
       </c>
       <c r="I24" s="85"/>
@@ -5038,7 +4959,7 @@
       <c r="F25" s="18"/>
       <c r="G25" s="1"/>
       <c r="H25" s="18">
-        <f>Général!H144</f>
+        <f>Général!H143</f>
         <v>0</v>
       </c>
       <c r="I25" s="85"/>
@@ -5062,7 +4983,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="1"/>
       <c r="H26" s="16">
-        <f>Général!H146</f>
+        <f>Général!H145</f>
         <v>0</v>
       </c>
       <c r="I26" s="85"/>
@@ -5086,7 +5007,7 @@
       <c r="F27" s="16"/>
       <c r="G27" s="1"/>
       <c r="H27" s="16">
-        <f>Général!H154</f>
+        <f>Général!H153</f>
         <v>0</v>
       </c>
       <c r="I27" s="85"/>
@@ -5110,7 +5031,7 @@
       <c r="F28" s="16"/>
       <c r="G28" s="1"/>
       <c r="H28" s="16">
-        <f>Général!H161</f>
+        <f>Général!H160</f>
         <v>0</v>
       </c>
       <c r="I28" s="85"/>
@@ -5134,7 +5055,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="1"/>
       <c r="H29" s="16">
-        <f>Général!H169</f>
+        <f>Général!H168</f>
         <v>0</v>
       </c>
       <c r="I29" s="85"/>
@@ -5158,7 +5079,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="1"/>
       <c r="H30" s="16">
-        <f>Général!H172</f>
+        <f>Général!H171</f>
         <v>0</v>
       </c>
       <c r="I30" s="85"/>
@@ -5182,7 +5103,7 @@
       <c r="F31" s="16"/>
       <c r="G31" s="1"/>
       <c r="H31" s="16">
-        <f>Général!H175</f>
+        <f>Général!H174</f>
         <v>0</v>
       </c>
       <c r="I31" s="85"/>
@@ -5206,7 +5127,7 @@
       <c r="F32" s="16"/>
       <c r="G32" s="1"/>
       <c r="H32" s="16">
-        <f>Général!H177</f>
+        <f>Général!H176</f>
         <v>0</v>
       </c>
       <c r="I32" s="85"/>
@@ -5230,7 +5151,7 @@
       <c r="F33" s="16"/>
       <c r="G33" s="1"/>
       <c r="H33" s="16">
-        <f>Général!H180</f>
+        <f>Général!H179</f>
         <v>0</v>
       </c>
       <c r="I33" s="85"/>
@@ -5254,7 +5175,7 @@
       <c r="F34" s="16"/>
       <c r="G34" s="1"/>
       <c r="H34" s="16">
-        <f>Général!H183</f>
+        <f>Général!H182</f>
         <v>0</v>
       </c>
       <c r="I34" s="85"/>
@@ -5278,7 +5199,7 @@
       <c r="F35" s="16"/>
       <c r="G35" s="1"/>
       <c r="H35" s="16">
-        <f>Général!H186</f>
+        <f>Général!H185</f>
         <v>0</v>
       </c>
       <c r="I35" s="85"/>
@@ -5302,7 +5223,7 @@
       <c r="F36" s="16"/>
       <c r="G36" s="1"/>
       <c r="H36" s="16">
-        <f>Général!H188</f>
+        <f>Général!H187</f>
         <v>0</v>
       </c>
       <c r="I36" s="85"/>
@@ -5326,7 +5247,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="1"/>
       <c r="H37" s="16">
-        <f>Général!H190</f>
+        <f>Général!H189</f>
         <v>0</v>
       </c>
       <c r="I37" s="85"/>
@@ -5350,7 +5271,7 @@
       <c r="F38" s="16"/>
       <c r="G38" s="1"/>
       <c r="H38" s="16">
-        <f>Général!H192</f>
+        <f>Général!H191</f>
         <v>0</v>
       </c>
       <c r="I38" s="85"/>
@@ -5374,7 +5295,7 @@
       <c r="F39" s="16"/>
       <c r="G39" s="1"/>
       <c r="H39" s="16">
-        <f>Général!H196</f>
+        <f>Général!H195</f>
         <v>0</v>
       </c>
       <c r="I39" s="85"/>
@@ -5398,7 +5319,7 @@
       <c r="F40" s="16"/>
       <c r="G40" s="1"/>
       <c r="H40" s="16">
-        <f>Général!H198</f>
+        <f>Général!H197</f>
         <v>0</v>
       </c>
       <c r="I40" s="85"/>
@@ -5422,7 +5343,7 @@
       <c r="F41" s="16"/>
       <c r="G41" s="1"/>
       <c r="H41" s="16">
-        <f>Général!H200</f>
+        <f>Général!H199</f>
         <v>0</v>
       </c>
       <c r="I41" s="85"/>
@@ -5446,7 +5367,7 @@
       <c r="F42" s="16"/>
       <c r="G42" s="1"/>
       <c r="H42" s="16">
-        <f>Général!H204</f>
+        <f>Général!H203</f>
         <v>0</v>
       </c>
       <c r="I42" s="85"/>
@@ -5470,7 +5391,7 @@
       <c r="F43" s="16"/>
       <c r="G43" s="1"/>
       <c r="H43" s="16">
-        <f>Général!H205</f>
+        <f>Général!H204</f>
         <v>0</v>
       </c>
       <c r="I43" s="85"/>
@@ -5571,7 +5492,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="16">
-        <f>Général!H101</f>
+        <f>Général!H100</f>
         <v>0</v>
       </c>
       <c r="I2" s="16"/>
@@ -5595,7 +5516,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="6"/>
       <c r="H3" s="19">
-        <f>Général!H102</f>
+        <f>Général!H101</f>
         <v>0</v>
       </c>
       <c r="I3" s="19"/>
@@ -5621,7 +5542,7 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="37">
-        <f>Général!H111</f>
+        <f>Général!H110</f>
         <v>0</v>
       </c>
       <c r="I4" s="19"/>
@@ -5645,7 +5566,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="2"/>
       <c r="H5" s="16">
-        <f>Général!H114</f>
+        <f>Général!H113</f>
         <v>0</v>
       </c>
       <c r="I5" s="16"/>
@@ -5669,7 +5590,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="2"/>
       <c r="H6" s="16">
-        <f>Général!H116</f>
+        <f>Général!H115</f>
         <v>0</v>
       </c>
       <c r="I6" s="16"/>
@@ -5693,7 +5614,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="2"/>
       <c r="H7" s="16">
-        <f>Général!H119</f>
+        <f>Général!H118</f>
         <v>0</v>
       </c>
       <c r="I7" s="16"/>
@@ -5717,7 +5638,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="6"/>
       <c r="H8" s="19">
-        <f>Général!H120</f>
+        <f>Général!H119</f>
         <v>0</v>
       </c>
       <c r="I8" s="19"/>
@@ -5741,7 +5662,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="9"/>
       <c r="H9" s="18">
-        <f>Général!H150</f>
+        <f>Général!H149</f>
         <v>0</v>
       </c>
       <c r="I9" s="18"/>
@@ -5765,7 +5686,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="2"/>
       <c r="H10" s="16">
-        <f>Général!H157</f>
+        <f>Général!H156</f>
         <v>0</v>
       </c>
       <c r="I10" s="16"/>
@@ -5791,7 +5712,7 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="16">
-        <f>Général!H164</f>
+        <f>Général!H163</f>
         <v>0</v>
       </c>
       <c r="I11" s="16"/>
@@ -5815,7 +5736,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="2"/>
       <c r="H12" s="16">
-        <f>Général!H165</f>
+        <f>Général!H164</f>
         <v>0</v>
       </c>
       <c r="I12" s="16"/>

</xml_diff>